<commit_message>
Updated the meeting minutes
</commit_message>
<xml_diff>
--- a/Sprint 2/Meeting Minutes/Meeting_Minutes_Sprint_2.xlsx
+++ b/Sprint 2/Meeting Minutes/Meeting_Minutes_Sprint_2.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carla\Desktop\341-project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carla\Desktop\341-project\ctrl_c_ctrl_v-SOEN341_Project_F24\Sprint 2\Meeting Minutes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DC40A17D-84E7-4DDB-9697-5A8673A3993F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B70B976F-EAB5-4320-BD35-5B65772A7190}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{1BA0CD9A-B9E0-48D4-86D3-C9682EC1275D}"/>
   </bookViews>
@@ -25,15 +25,74 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="20">
   <si>
     <t>Daily Scrum</t>
   </si>
   <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>time</t>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>Attendees</t>
+  </si>
+  <si>
+    <t>Agenda</t>
+  </si>
+  <si>
+    <t>Discussion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">October 3rd, 2024 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">4:15pm - 4:30pm </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Concordia University H8 Lab Room  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mauricio Murillo,  
+Rym Dallali,  
+Nolan Ganz,  
+Khalil Labban,  
+Jaden Wright-Maurais,  
+Carla Chamandi  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">During this meeting, we reviewed the user stories and tasks currently in progress. We ensured that each team member had a clear understanding of their responsibilities and the next steps for the project.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">October 5th, 2024  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">11:00pm - 11:15:pm </t>
+  </si>
+  <si>
+    <t>Discord</t>
+  </si>
+  <si>
+    <t>1) Input validation
+2) Table creation for courses and teams</t>
+  </si>
+  <si>
+    <t>1) Go over user stories and tasks</t>
+  </si>
+  <si>
+    <t>In this meeting, we focused on updating the input validation for account creation on both the frontend and backend. Additionally, we created a table for courses and updated the functionality so that teams could be attached to a course, streamlining the data structure for future use.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">October 9th, 2024 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) Fetch module clarification  
+2) Project modifications  </t>
+  </si>
+  <si>
+    <t>We discussed the fetch module and clarified its usage within the project. Additionally, we decided to remove the username field from the project as it was no longer necessary based on the updated requirements.</t>
   </si>
 </sst>
 </file>
@@ -69,8 +128,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -385,15 +450,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0ADACE44-A1BC-47E6-A04D-E724ACE2BBAC}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:J100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="22.33203125" customWidth="1"/>
+    <col min="2" max="2" width="18" customWidth="1"/>
+    <col min="3" max="3" width="34.109375" customWidth="1"/>
+    <col min="4" max="4" width="26.109375" customWidth="1"/>
+    <col min="5" max="5" width="30.6640625" customWidth="1"/>
+    <col min="6" max="6" width="40.109375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -403,6 +476,1251 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="83.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+    </row>
+    <row r="3" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+    </row>
+    <row r="4" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+    </row>
+    <row r="5" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="1"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+    </row>
+    <row r="6" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="1"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+    </row>
+    <row r="7" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="1"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+      <c r="J26" s="1"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
+      <c r="J27" s="1"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+      <c r="J28" s="1"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
+      <c r="J29" s="1"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A30" s="1"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
+      <c r="I30" s="1"/>
+      <c r="J30" s="1"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A31" s="1"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+      <c r="H31" s="1"/>
+      <c r="I31" s="1"/>
+      <c r="J31" s="1"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A32" s="1"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
+      <c r="H32" s="1"/>
+      <c r="I32" s="1"/>
+      <c r="J32" s="1"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A33" s="1"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
+      <c r="H33" s="1"/>
+      <c r="I33" s="1"/>
+      <c r="J33" s="1"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A34" s="1"/>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1"/>
+      <c r="G34" s="1"/>
+      <c r="H34" s="1"/>
+      <c r="I34" s="1"/>
+      <c r="J34" s="1"/>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A35" s="1"/>
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+      <c r="F35" s="1"/>
+      <c r="G35" s="1"/>
+      <c r="H35" s="1"/>
+      <c r="I35" s="1"/>
+      <c r="J35" s="1"/>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A36" s="1"/>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
+      <c r="G36" s="1"/>
+      <c r="H36" s="1"/>
+      <c r="I36" s="1"/>
+      <c r="J36" s="1"/>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A37" s="1"/>
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1"/>
+      <c r="G37" s="1"/>
+      <c r="H37" s="1"/>
+      <c r="I37" s="1"/>
+      <c r="J37" s="1"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A38" s="1"/>
+      <c r="B38" s="1"/>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+      <c r="F38" s="1"/>
+      <c r="G38" s="1"/>
+      <c r="H38" s="1"/>
+      <c r="I38" s="1"/>
+      <c r="J38" s="1"/>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A39" s="1"/>
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+      <c r="F39" s="1"/>
+      <c r="G39" s="1"/>
+      <c r="H39" s="1"/>
+      <c r="I39" s="1"/>
+      <c r="J39" s="1"/>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A40" s="1"/>
+      <c r="B40" s="1"/>
+      <c r="C40" s="1"/>
+      <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
+      <c r="F40" s="1"/>
+      <c r="G40" s="1"/>
+      <c r="H40" s="1"/>
+      <c r="I40" s="1"/>
+      <c r="J40" s="1"/>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A41" s="1"/>
+      <c r="B41" s="1"/>
+      <c r="C41" s="1"/>
+      <c r="D41" s="1"/>
+      <c r="E41" s="1"/>
+      <c r="F41" s="1"/>
+      <c r="G41" s="1"/>
+      <c r="H41" s="1"/>
+      <c r="I41" s="1"/>
+      <c r="J41" s="1"/>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A42" s="1"/>
+      <c r="B42" s="1"/>
+      <c r="C42" s="1"/>
+      <c r="D42" s="1"/>
+      <c r="E42" s="1"/>
+      <c r="F42" s="1"/>
+      <c r="G42" s="1"/>
+      <c r="H42" s="1"/>
+      <c r="I42" s="1"/>
+      <c r="J42" s="1"/>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A43" s="1"/>
+      <c r="B43" s="1"/>
+      <c r="C43" s="1"/>
+      <c r="D43" s="1"/>
+      <c r="E43" s="1"/>
+      <c r="F43" s="1"/>
+      <c r="G43" s="1"/>
+      <c r="H43" s="1"/>
+      <c r="I43" s="1"/>
+      <c r="J43" s="1"/>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A44" s="1"/>
+      <c r="B44" s="1"/>
+      <c r="C44" s="1"/>
+      <c r="D44" s="1"/>
+      <c r="E44" s="1"/>
+      <c r="F44" s="1"/>
+      <c r="G44" s="1"/>
+      <c r="H44" s="1"/>
+      <c r="I44" s="1"/>
+      <c r="J44" s="1"/>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A45" s="1"/>
+      <c r="B45" s="1"/>
+      <c r="C45" s="1"/>
+      <c r="D45" s="1"/>
+      <c r="E45" s="1"/>
+      <c r="F45" s="1"/>
+      <c r="G45" s="1"/>
+      <c r="H45" s="1"/>
+      <c r="I45" s="1"/>
+      <c r="J45" s="1"/>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A46" s="1"/>
+      <c r="B46" s="1"/>
+      <c r="C46" s="1"/>
+      <c r="D46" s="1"/>
+      <c r="E46" s="1"/>
+      <c r="F46" s="1"/>
+      <c r="G46" s="1"/>
+      <c r="H46" s="1"/>
+      <c r="I46" s="1"/>
+      <c r="J46" s="1"/>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A47" s="1"/>
+      <c r="B47" s="1"/>
+      <c r="C47" s="1"/>
+      <c r="D47" s="1"/>
+      <c r="E47" s="1"/>
+      <c r="F47" s="1"/>
+      <c r="G47" s="1"/>
+      <c r="H47" s="1"/>
+      <c r="I47" s="1"/>
+      <c r="J47" s="1"/>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A48" s="1"/>
+      <c r="B48" s="1"/>
+      <c r="C48" s="1"/>
+      <c r="D48" s="1"/>
+      <c r="E48" s="1"/>
+      <c r="F48" s="1"/>
+      <c r="G48" s="1"/>
+      <c r="H48" s="1"/>
+      <c r="I48" s="1"/>
+      <c r="J48" s="1"/>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A49" s="1"/>
+      <c r="B49" s="1"/>
+      <c r="C49" s="1"/>
+      <c r="D49" s="1"/>
+      <c r="E49" s="1"/>
+      <c r="F49" s="1"/>
+      <c r="G49" s="1"/>
+      <c r="H49" s="1"/>
+      <c r="I49" s="1"/>
+      <c r="J49" s="1"/>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A50" s="1"/>
+      <c r="B50" s="1"/>
+      <c r="C50" s="1"/>
+      <c r="D50" s="1"/>
+      <c r="E50" s="1"/>
+      <c r="F50" s="1"/>
+      <c r="G50" s="1"/>
+      <c r="H50" s="1"/>
+      <c r="I50" s="1"/>
+      <c r="J50" s="1"/>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A51" s="1"/>
+      <c r="B51" s="1"/>
+      <c r="C51" s="1"/>
+      <c r="D51" s="1"/>
+      <c r="E51" s="1"/>
+      <c r="F51" s="1"/>
+      <c r="G51" s="1"/>
+      <c r="H51" s="1"/>
+      <c r="I51" s="1"/>
+      <c r="J51" s="1"/>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A52" s="1"/>
+      <c r="B52" s="1"/>
+      <c r="C52" s="1"/>
+      <c r="D52" s="1"/>
+      <c r="E52" s="1"/>
+      <c r="F52" s="1"/>
+      <c r="G52" s="1"/>
+      <c r="H52" s="1"/>
+      <c r="I52" s="1"/>
+      <c r="J52" s="1"/>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A53" s="1"/>
+      <c r="B53" s="1"/>
+      <c r="C53" s="1"/>
+      <c r="D53" s="1"/>
+      <c r="E53" s="1"/>
+      <c r="F53" s="1"/>
+      <c r="G53" s="1"/>
+      <c r="H53" s="1"/>
+      <c r="I53" s="1"/>
+      <c r="J53" s="1"/>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A54" s="1"/>
+      <c r="B54" s="1"/>
+      <c r="C54" s="1"/>
+      <c r="D54" s="1"/>
+      <c r="E54" s="1"/>
+      <c r="F54" s="1"/>
+      <c r="G54" s="1"/>
+      <c r="H54" s="1"/>
+      <c r="I54" s="1"/>
+      <c r="J54" s="1"/>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A55" s="1"/>
+      <c r="B55" s="1"/>
+      <c r="C55" s="1"/>
+      <c r="D55" s="1"/>
+      <c r="E55" s="1"/>
+      <c r="F55" s="1"/>
+      <c r="G55" s="1"/>
+      <c r="H55" s="1"/>
+      <c r="I55" s="1"/>
+      <c r="J55" s="1"/>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A56" s="1"/>
+      <c r="B56" s="1"/>
+      <c r="C56" s="1"/>
+      <c r="D56" s="1"/>
+      <c r="E56" s="1"/>
+      <c r="F56" s="1"/>
+      <c r="G56" s="1"/>
+      <c r="H56" s="1"/>
+      <c r="I56" s="1"/>
+      <c r="J56" s="1"/>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A57" s="1"/>
+      <c r="B57" s="1"/>
+      <c r="C57" s="1"/>
+      <c r="D57" s="1"/>
+      <c r="E57" s="1"/>
+      <c r="F57" s="1"/>
+      <c r="G57" s="1"/>
+      <c r="H57" s="1"/>
+      <c r="I57" s="1"/>
+      <c r="J57" s="1"/>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A58" s="1"/>
+      <c r="B58" s="1"/>
+      <c r="C58" s="1"/>
+      <c r="D58" s="1"/>
+      <c r="E58" s="1"/>
+      <c r="F58" s="1"/>
+      <c r="G58" s="1"/>
+      <c r="H58" s="1"/>
+      <c r="I58" s="1"/>
+      <c r="J58" s="1"/>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A59" s="1"/>
+      <c r="B59" s="1"/>
+      <c r="C59" s="1"/>
+      <c r="D59" s="1"/>
+      <c r="E59" s="1"/>
+      <c r="F59" s="1"/>
+      <c r="G59" s="1"/>
+      <c r="H59" s="1"/>
+      <c r="I59" s="1"/>
+      <c r="J59" s="1"/>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A60" s="1"/>
+      <c r="B60" s="1"/>
+      <c r="C60" s="1"/>
+      <c r="D60" s="1"/>
+      <c r="E60" s="1"/>
+      <c r="F60" s="1"/>
+      <c r="G60" s="1"/>
+      <c r="H60" s="1"/>
+      <c r="I60" s="1"/>
+      <c r="J60" s="1"/>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A61" s="1"/>
+      <c r="B61" s="1"/>
+      <c r="C61" s="1"/>
+      <c r="D61" s="1"/>
+      <c r="E61" s="1"/>
+      <c r="F61" s="1"/>
+      <c r="G61" s="1"/>
+      <c r="H61" s="1"/>
+      <c r="I61" s="1"/>
+      <c r="J61" s="1"/>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A62" s="1"/>
+      <c r="B62" s="1"/>
+      <c r="C62" s="1"/>
+      <c r="D62" s="1"/>
+      <c r="E62" s="1"/>
+      <c r="F62" s="1"/>
+      <c r="G62" s="1"/>
+      <c r="H62" s="1"/>
+      <c r="I62" s="1"/>
+      <c r="J62" s="1"/>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A63" s="1"/>
+      <c r="B63" s="1"/>
+      <c r="C63" s="1"/>
+      <c r="D63" s="1"/>
+      <c r="E63" s="1"/>
+      <c r="F63" s="1"/>
+      <c r="G63" s="1"/>
+      <c r="H63" s="1"/>
+      <c r="I63" s="1"/>
+      <c r="J63" s="1"/>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A64" s="1"/>
+      <c r="B64" s="1"/>
+      <c r="C64" s="1"/>
+      <c r="D64" s="1"/>
+      <c r="E64" s="1"/>
+      <c r="F64" s="1"/>
+      <c r="G64" s="1"/>
+      <c r="H64" s="1"/>
+      <c r="I64" s="1"/>
+      <c r="J64" s="1"/>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A65" s="1"/>
+      <c r="B65" s="1"/>
+      <c r="C65" s="1"/>
+      <c r="D65" s="1"/>
+      <c r="E65" s="1"/>
+      <c r="F65" s="1"/>
+      <c r="G65" s="1"/>
+      <c r="H65" s="1"/>
+      <c r="I65" s="1"/>
+      <c r="J65" s="1"/>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A66" s="1"/>
+      <c r="B66" s="1"/>
+      <c r="C66" s="1"/>
+      <c r="D66" s="1"/>
+      <c r="E66" s="1"/>
+      <c r="F66" s="1"/>
+      <c r="G66" s="1"/>
+      <c r="H66" s="1"/>
+      <c r="I66" s="1"/>
+      <c r="J66" s="1"/>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A67" s="1"/>
+      <c r="B67" s="1"/>
+      <c r="C67" s="1"/>
+      <c r="D67" s="1"/>
+      <c r="E67" s="1"/>
+      <c r="F67" s="1"/>
+      <c r="G67" s="1"/>
+      <c r="H67" s="1"/>
+      <c r="I67" s="1"/>
+      <c r="J67" s="1"/>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A68" s="1"/>
+      <c r="B68" s="1"/>
+      <c r="C68" s="1"/>
+      <c r="D68" s="1"/>
+      <c r="E68" s="1"/>
+      <c r="F68" s="1"/>
+      <c r="G68" s="1"/>
+      <c r="H68" s="1"/>
+      <c r="I68" s="1"/>
+      <c r="J68" s="1"/>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A69" s="1"/>
+      <c r="B69" s="1"/>
+      <c r="C69" s="1"/>
+      <c r="D69" s="1"/>
+      <c r="E69" s="1"/>
+      <c r="F69" s="1"/>
+      <c r="G69" s="1"/>
+      <c r="H69" s="1"/>
+      <c r="I69" s="1"/>
+      <c r="J69" s="1"/>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A70" s="1"/>
+      <c r="B70" s="1"/>
+      <c r="C70" s="1"/>
+      <c r="D70" s="1"/>
+      <c r="E70" s="1"/>
+      <c r="F70" s="1"/>
+      <c r="G70" s="1"/>
+      <c r="H70" s="1"/>
+      <c r="I70" s="1"/>
+      <c r="J70" s="1"/>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A71" s="1"/>
+      <c r="B71" s="1"/>
+      <c r="C71" s="1"/>
+      <c r="D71" s="1"/>
+      <c r="E71" s="1"/>
+      <c r="F71" s="1"/>
+      <c r="G71" s="1"/>
+      <c r="H71" s="1"/>
+      <c r="I71" s="1"/>
+      <c r="J71" s="1"/>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A72" s="1"/>
+      <c r="B72" s="1"/>
+      <c r="C72" s="1"/>
+      <c r="D72" s="1"/>
+      <c r="E72" s="1"/>
+      <c r="F72" s="1"/>
+      <c r="G72" s="1"/>
+      <c r="H72" s="1"/>
+      <c r="I72" s="1"/>
+      <c r="J72" s="1"/>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A73" s="1"/>
+      <c r="B73" s="1"/>
+      <c r="C73" s="1"/>
+      <c r="D73" s="1"/>
+      <c r="E73" s="1"/>
+      <c r="F73" s="1"/>
+      <c r="G73" s="1"/>
+      <c r="H73" s="1"/>
+      <c r="I73" s="1"/>
+      <c r="J73" s="1"/>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A74" s="1"/>
+      <c r="B74" s="1"/>
+      <c r="C74" s="1"/>
+      <c r="D74" s="1"/>
+      <c r="E74" s="1"/>
+      <c r="F74" s="1"/>
+      <c r="G74" s="1"/>
+      <c r="H74" s="1"/>
+      <c r="I74" s="1"/>
+      <c r="J74" s="1"/>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A75" s="1"/>
+      <c r="B75" s="1"/>
+      <c r="C75" s="1"/>
+      <c r="D75" s="1"/>
+      <c r="E75" s="1"/>
+      <c r="F75" s="1"/>
+      <c r="G75" s="1"/>
+      <c r="H75" s="1"/>
+      <c r="I75" s="1"/>
+      <c r="J75" s="1"/>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A76" s="1"/>
+      <c r="B76" s="1"/>
+      <c r="C76" s="1"/>
+      <c r="D76" s="1"/>
+      <c r="E76" s="1"/>
+      <c r="F76" s="1"/>
+      <c r="G76" s="1"/>
+      <c r="H76" s="1"/>
+      <c r="I76" s="1"/>
+      <c r="J76" s="1"/>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A77" s="1"/>
+      <c r="B77" s="1"/>
+      <c r="C77" s="1"/>
+      <c r="D77" s="1"/>
+      <c r="E77" s="1"/>
+      <c r="F77" s="1"/>
+      <c r="G77" s="1"/>
+      <c r="H77" s="1"/>
+      <c r="I77" s="1"/>
+      <c r="J77" s="1"/>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A78" s="1"/>
+      <c r="B78" s="1"/>
+      <c r="C78" s="1"/>
+      <c r="D78" s="1"/>
+      <c r="E78" s="1"/>
+      <c r="F78" s="1"/>
+      <c r="G78" s="1"/>
+      <c r="H78" s="1"/>
+      <c r="I78" s="1"/>
+      <c r="J78" s="1"/>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A79" s="1"/>
+      <c r="B79" s="1"/>
+      <c r="C79" s="1"/>
+      <c r="D79" s="1"/>
+      <c r="E79" s="1"/>
+      <c r="F79" s="1"/>
+      <c r="G79" s="1"/>
+      <c r="H79" s="1"/>
+      <c r="I79" s="1"/>
+      <c r="J79" s="1"/>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A80" s="1"/>
+      <c r="B80" s="1"/>
+      <c r="C80" s="1"/>
+      <c r="D80" s="1"/>
+      <c r="E80" s="1"/>
+      <c r="F80" s="1"/>
+      <c r="G80" s="1"/>
+      <c r="H80" s="1"/>
+      <c r="I80" s="1"/>
+      <c r="J80" s="1"/>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A81" s="1"/>
+      <c r="B81" s="1"/>
+      <c r="C81" s="1"/>
+      <c r="D81" s="1"/>
+      <c r="E81" s="1"/>
+      <c r="F81" s="1"/>
+      <c r="G81" s="1"/>
+      <c r="H81" s="1"/>
+      <c r="I81" s="1"/>
+      <c r="J81" s="1"/>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A82" s="1"/>
+      <c r="B82" s="1"/>
+      <c r="C82" s="1"/>
+      <c r="D82" s="1"/>
+      <c r="E82" s="1"/>
+      <c r="F82" s="1"/>
+      <c r="G82" s="1"/>
+      <c r="H82" s="1"/>
+      <c r="I82" s="1"/>
+      <c r="J82" s="1"/>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A83" s="1"/>
+      <c r="B83" s="1"/>
+      <c r="C83" s="1"/>
+      <c r="D83" s="1"/>
+      <c r="E83" s="1"/>
+      <c r="F83" s="1"/>
+      <c r="G83" s="1"/>
+      <c r="H83" s="1"/>
+      <c r="I83" s="1"/>
+      <c r="J83" s="1"/>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A84" s="1"/>
+      <c r="B84" s="1"/>
+      <c r="C84" s="1"/>
+      <c r="D84" s="1"/>
+      <c r="E84" s="1"/>
+      <c r="F84" s="1"/>
+      <c r="G84" s="1"/>
+      <c r="H84" s="1"/>
+      <c r="I84" s="1"/>
+      <c r="J84" s="1"/>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A85" s="1"/>
+      <c r="B85" s="1"/>
+      <c r="C85" s="1"/>
+      <c r="D85" s="1"/>
+      <c r="E85" s="1"/>
+      <c r="F85" s="1"/>
+      <c r="G85" s="1"/>
+      <c r="H85" s="1"/>
+      <c r="I85" s="1"/>
+      <c r="J85" s="1"/>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A86" s="1"/>
+      <c r="B86" s="1"/>
+      <c r="C86" s="1"/>
+      <c r="D86" s="1"/>
+      <c r="E86" s="1"/>
+      <c r="F86" s="1"/>
+      <c r="G86" s="1"/>
+      <c r="H86" s="1"/>
+      <c r="I86" s="1"/>
+      <c r="J86" s="1"/>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A87" s="1"/>
+      <c r="B87" s="1"/>
+      <c r="C87" s="1"/>
+      <c r="D87" s="1"/>
+      <c r="E87" s="1"/>
+      <c r="F87" s="1"/>
+      <c r="G87" s="1"/>
+      <c r="H87" s="1"/>
+      <c r="I87" s="1"/>
+      <c r="J87" s="1"/>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A88" s="1"/>
+      <c r="B88" s="1"/>
+      <c r="C88" s="1"/>
+      <c r="D88" s="1"/>
+      <c r="E88" s="1"/>
+      <c r="F88" s="1"/>
+      <c r="G88" s="1"/>
+      <c r="H88" s="1"/>
+      <c r="I88" s="1"/>
+      <c r="J88" s="1"/>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A89" s="1"/>
+      <c r="B89" s="1"/>
+      <c r="C89" s="1"/>
+      <c r="D89" s="1"/>
+      <c r="E89" s="1"/>
+      <c r="F89" s="1"/>
+      <c r="G89" s="1"/>
+      <c r="H89" s="1"/>
+      <c r="I89" s="1"/>
+      <c r="J89" s="1"/>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A90" s="1"/>
+      <c r="B90" s="1"/>
+      <c r="C90" s="1"/>
+      <c r="D90" s="1"/>
+      <c r="E90" s="1"/>
+      <c r="F90" s="1"/>
+      <c r="G90" s="1"/>
+      <c r="H90" s="1"/>
+      <c r="I90" s="1"/>
+      <c r="J90" s="1"/>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A91" s="1"/>
+      <c r="B91" s="1"/>
+      <c r="C91" s="1"/>
+      <c r="D91" s="1"/>
+      <c r="E91" s="1"/>
+      <c r="F91" s="1"/>
+      <c r="G91" s="1"/>
+      <c r="H91" s="1"/>
+      <c r="I91" s="1"/>
+      <c r="J91" s="1"/>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A92" s="1"/>
+      <c r="B92" s="1"/>
+      <c r="C92" s="1"/>
+      <c r="D92" s="1"/>
+      <c r="E92" s="1"/>
+      <c r="F92" s="1"/>
+      <c r="G92" s="1"/>
+      <c r="H92" s="1"/>
+      <c r="I92" s="1"/>
+      <c r="J92" s="1"/>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A93" s="1"/>
+      <c r="B93" s="1"/>
+      <c r="C93" s="1"/>
+      <c r="D93" s="1"/>
+      <c r="E93" s="1"/>
+      <c r="F93" s="1"/>
+      <c r="G93" s="1"/>
+      <c r="H93" s="1"/>
+      <c r="I93" s="1"/>
+      <c r="J93" s="1"/>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A94" s="1"/>
+      <c r="B94" s="1"/>
+      <c r="C94" s="1"/>
+      <c r="D94" s="1"/>
+      <c r="E94" s="1"/>
+      <c r="F94" s="1"/>
+      <c r="G94" s="1"/>
+      <c r="H94" s="1"/>
+      <c r="I94" s="1"/>
+      <c r="J94" s="1"/>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A95" s="1"/>
+      <c r="B95" s="1"/>
+      <c r="C95" s="1"/>
+      <c r="D95" s="1"/>
+      <c r="E95" s="1"/>
+      <c r="F95" s="1"/>
+      <c r="G95" s="1"/>
+      <c r="H95" s="1"/>
+      <c r="I95" s="1"/>
+      <c r="J95" s="1"/>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A96" s="1"/>
+      <c r="B96" s="1"/>
+      <c r="C96" s="1"/>
+      <c r="D96" s="1"/>
+      <c r="E96" s="1"/>
+      <c r="F96" s="1"/>
+      <c r="G96" s="1"/>
+      <c r="H96" s="1"/>
+      <c r="I96" s="1"/>
+      <c r="J96" s="1"/>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A97" s="1"/>
+      <c r="B97" s="1"/>
+      <c r="C97" s="1"/>
+      <c r="D97" s="1"/>
+      <c r="E97" s="1"/>
+      <c r="F97" s="1"/>
+      <c r="G97" s="1"/>
+      <c r="H97" s="1"/>
+      <c r="I97" s="1"/>
+      <c r="J97" s="1"/>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A98" s="1"/>
+      <c r="B98" s="1"/>
+      <c r="C98" s="1"/>
+      <c r="D98" s="1"/>
+      <c r="E98" s="1"/>
+      <c r="F98" s="1"/>
+      <c r="G98" s="1"/>
+      <c r="H98" s="1"/>
+      <c r="I98" s="1"/>
+      <c r="J98" s="1"/>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A99" s="1"/>
+      <c r="B99" s="1"/>
+      <c r="C99" s="1"/>
+      <c r="D99" s="1"/>
+      <c r="E99" s="1"/>
+      <c r="F99" s="1"/>
+      <c r="G99" s="1"/>
+      <c r="H99" s="1"/>
+      <c r="I99" s="1"/>
+      <c r="J99" s="1"/>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A100" s="1"/>
+      <c r="B100" s="1"/>
+      <c r="C100" s="1"/>
+      <c r="D100" s="1"/>
+      <c r="E100" s="1"/>
+      <c r="F100" s="1"/>
+      <c r="G100" s="1"/>
+      <c r="H100" s="1"/>
+      <c r="I100" s="1"/>
+      <c r="J100" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated the daily scrums
</commit_message>
<xml_diff>
--- a/Sprint 2/Meeting Minutes/Meeting_Minutes_Sprint_2.xlsx
+++ b/Sprint 2/Meeting Minutes/Meeting_Minutes_Sprint_2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carla\Desktop\341-project\ctrl_c_ctrl_v-SOEN341_Project_F24\Sprint 2\Meeting Minutes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20083345-26D6-407D-894D-BCD59221418A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E6346F5-3FAA-4338-9958-AF6017156281}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="11772" windowHeight="12336" xr2:uid="{1BA0CD9A-B9E0-48D4-86D3-C9682EC1275D}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{1BA0CD9A-B9E0-48D4-86D3-C9682EC1275D}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -79,16 +79,10 @@
     <t>1) Go over user stories and tasks</t>
   </si>
   <si>
-    <t>In this meeting, we focused on updating the input validation for account creation on both the frontend and backend. Additionally, we created a table for courses and updated the functionality so that teams could be attached to a course, streamlining the data structure for future use.</t>
-  </si>
-  <si>
     <t xml:space="preserve">1) Fetch module clarification  
 2) Project modifications  </t>
   </si>
   <si>
-    <t>We discussed the fetch module and clarified its usage within the project. Additionally, we decided to remove the username field from the project as it was no longer necessary based on the updated requirements.</t>
-  </si>
-  <si>
     <t xml:space="preserve">October 7th, 2024 </t>
   </si>
   <si>
@@ -96,9 +90,6 @@
   </si>
   <si>
     <t>1)UI design for students' view</t>
-  </si>
-  <si>
-    <t>We began work on the UI design for the students’ view, focusing on creating an intuitive layout to improve user experience. The team discussed initial design choices and planned further enhancements.</t>
   </si>
   <si>
     <t xml:space="preserve">October 8th, 2024 </t>
@@ -108,26 +99,16 @@
 2) User verification logic </t>
   </si>
   <si>
-    <t>We worked on creating the Teams API and successfully added tests for the functionality. In addition, we implemented some logic for user verification to ensure that only authorized users can perform specific actions within the system.</t>
-  </si>
-  <si>
     <t>October 11th, 2024</t>
   </si>
   <si>
     <t>1) Continuation of UI design for students' view</t>
   </si>
   <si>
-    <t>We continued refining the UI design for the students’ view, finalizing adjustments to make the layout more user-friendly. The team ensured alignment on the design vision and began preparations for implementation.</t>
-  </si>
-  <si>
     <t xml:space="preserve">October 13th, 2024  </t>
   </si>
   <si>
     <t xml:space="preserve">1) Backend and frontend updates  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">During this meeting, we worked on backend endpoints to retrieve courses and further developed the teams page. We also reviewed a pull request to ensure that the changes aligned with the project requirements.
-</t>
   </si>
   <si>
     <t xml:space="preserve">October 14th-15th, 2024 </t>
@@ -140,9 +121,6 @@
 2) CSV upload page</t>
   </si>
   <si>
-    <t>We focused on implementing the instructor’s student list functionality and worked on the frontend CSV upload page. Additionally, we clarified the team information that should be sent to the frontend and enforced database rules to ensure that each student is part of only one team.</t>
-  </si>
-  <si>
     <t xml:space="preserve">October 16th-17th, 2024  </t>
   </si>
   <si>
@@ -150,9 +128,6 @@
 2) Team CRUD  </t>
   </si>
   <si>
-    <t>We began working on course selection functionality and continued developing the team CRUD (Create, Read, Update, Delete) features. In addition, we fixed bugs and implemented course selection binding, along with logic for student views. Acceptance tests were performed for the login and registration processes, and we started working on teammate evaluation UI and logic.</t>
-  </si>
-  <si>
     <t xml:space="preserve">October 18th, 2024  </t>
   </si>
   <si>
@@ -175,10 +150,6 @@
 2) UI design for team creation  </t>
   </si>
   <si>
-    <t xml:space="preserve">We continued learning about APIs and worked together to help improve the UI design of the CSV drag and drop feature. Progress was also made on the design of the team creation page.
-</t>
-  </si>
-  <si>
     <t>October 19th, 2024</t>
   </si>
   <si>
@@ -189,9 +160,6 @@
 2) Test fixes</t>
   </si>
   <si>
-    <t>We focused on merging pending pull requests and fixing issues with existing tests. Additionally, we reviewed what tasks remained for the sprint and aligned team members on priorities to ensure all critical items are addressed.</t>
-  </si>
-  <si>
     <t>October 21st, 2024</t>
   </si>
   <si>
@@ -202,10 +170,6 @@
 2) CI pipeline debugging</t>
   </si>
   <si>
-    <t xml:space="preserve">The team continued working on the team creation page, refining the design and implementation. We also dedicated time to debugging the CI pipeline to improve its stability and efficiency for ongoing development needs.
-</t>
-  </si>
-  <si>
     <t xml:space="preserve">October 22nd-23rd, 2024 </t>
   </si>
   <si>
@@ -213,9 +177,6 @@
 2) Members page implementation  </t>
   </si>
   <si>
-    <t>During these meetings, we completed the evaluations endpoints and reviewed multiple pull requests. We helped debug some issues and finished the implementation of the members page, connecting it to the necessary APIs. The CSV upload page was also connected to the backend successfully.</t>
-  </si>
-  <si>
     <t xml:space="preserve">October 24th, 2024  </t>
   </si>
   <si>
@@ -225,7 +186,51 @@
     <t xml:space="preserve">1) Task separation and sprint planning  </t>
   </si>
   <si>
-    <t>We discussed the separation of tasks for the remaining work in the sprint. We also talked about how to use context effectively, the grading structure, and the timing of the tasks. Each team member committed to completing their assigned tasks by the end of the sprint.</t>
+    <t>The team reviewed recent updates to input validation for account creation, addressing any outstanding issues. We also discussed the approach for organizing data tables for courses and teams to ensure clarity and maintainability in the project structure.</t>
+  </si>
+  <si>
+    <t>We discussed initial design ideas for the students’ view interface, focusing on layout and user experience considerations. Feedback was shared on each design approach, and we outlined next steps for creating a cohesive look.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The team discussed the functionality and use cases of the fetch module in our project. We also reviewed the decision to remove usernames to simplify the database structure and reduce redundancy.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We finalized the design choices for the students' view UI, discussing adjustments to ensure the interface was both user-friendly and aligned with our initial vision. We agreed on key elements to focus on during implementation.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We discussed the progress of the Teams API, including the approach to testing and verifying it. Additionally, the team deliberated on the best approach to implementing user verification to ensure secure data handling.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We reviewed the new backend endpoints for fetching course data and discussed updates to the teams page. We also reviewed the pull request process to confirm alignment with project requirements and discussed future improvements for smoother integration.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We discussed the design and implementation plan for the instructor's student list and reviewed the frontend interface for the CSV upload page. Team members shared insights on database rules to enforce team restrictions, which we agreed to implement in the upcoming days.
+</t>
+  </si>
+  <si>
+    <t>We discussed the development of the course selection functionality, with an emphasis on improving user experience. Team members also reviewed the current status of the team CRUD operations, shared feedback on acceptance testing, and brainstormed UI improvements for teammate evaluation.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The team explored strategies for integrating APIs effectively. We also reviewed the current design for the team creation page and discussed adjustments to improve clarity and usability.
+</t>
+  </si>
+  <si>
+    <t>We discussed the strategy for merging pull requests, including handling conflicts and managing test fixes. Team members shared insights on efficient testing practices, which will streamline the integration process.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We discussed the final adjustments needed for the team creation page and reviewed issues with the CI pipeline, proposing debugging steps to improve stability for ongoing development.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The team discussed the requirements for the evaluations endpoints and reviewed their integration with the frontend. We also examined the remaining steps for the members page implementation and proposed final modifications for the CSV upload functionality.
+</t>
+  </si>
+  <si>
+    <t>The team discussed the separation of tasks for the remainder of the sprint, including reviewing commitments and setting realistic deadlines. We also addressed any concerns with task timing and how to leverage context for a more organized workflow.</t>
   </si>
 </sst>
 </file>
@@ -591,8 +596,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0ADACE44-A1BC-47E6-A04D-E724ACE2BBAC}">
   <dimension ref="A1:J100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" topLeftCell="D13" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -649,12 +654,12 @@
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
     </row>
-    <row r="3" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>12</v>
@@ -666,7 +671,7 @@
         <v>13</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>15</v>
+        <v>48</v>
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
@@ -675,10 +680,10 @@
     </row>
     <row r="4" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>12</v>
@@ -687,10 +692,10 @@
         <v>9</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>21</v>
+        <v>49</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
@@ -699,10 +704,10 @@
     </row>
     <row r="5" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>12</v>
@@ -711,10 +716,10 @@
         <v>9</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>24</v>
+        <v>52</v>
       </c>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
@@ -723,10 +728,10 @@
     </row>
     <row r="6" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>12</v>
@@ -735,10 +740,10 @@
         <v>9</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>17</v>
+        <v>50</v>
       </c>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
@@ -747,10 +752,10 @@
     </row>
     <row r="7" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>12</v>
@@ -759,22 +764,22 @@
         <v>9</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>27</v>
+        <v>51</v>
       </c>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
     </row>
-    <row r="8" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>12</v>
@@ -783,22 +788,22 @@
         <v>9</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>30</v>
+        <v>53</v>
       </c>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
     </row>
-    <row r="9" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>12</v>
@@ -807,22 +812,22 @@
         <v>9</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>34</v>
+        <v>54</v>
       </c>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
     </row>
-    <row r="10" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>8</v>
@@ -831,22 +836,22 @@
         <v>9</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>37</v>
+        <v>55</v>
       </c>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
     </row>
-    <row r="11" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>12</v>
@@ -855,10 +860,10 @@
         <v>9</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
@@ -867,10 +872,10 @@
     </row>
     <row r="12" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>12</v>
@@ -879,10 +884,10 @@
         <v>9</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
@@ -891,10 +896,10 @@
     </row>
     <row r="13" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>12</v>
@@ -903,22 +908,22 @@
         <v>9</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
     </row>
-    <row r="14" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>12</v>
@@ -927,10 +932,10 @@
         <v>9</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
@@ -939,10 +944,10 @@
     </row>
     <row r="15" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>8</v>
@@ -951,7 +956,7 @@
         <v>9</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>60</v>

</xml_diff>

<commit_message>
Fixed the meeting minutes
</commit_message>
<xml_diff>
--- a/Sprint 2/Meeting Minutes/Meeting_Minutes_Sprint_2.xlsx
+++ b/Sprint 2/Meeting Minutes/Meeting_Minutes_Sprint_2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carla\Desktop\341-project\ctrl_c_ctrl_v-SOEN341_Project_F24\Sprint 2\Meeting Minutes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E6346F5-3FAA-4338-9958-AF6017156281}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B808F01C-6F8F-46D3-8CA2-C129F4E18C40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{1BA0CD9A-B9E0-48D4-86D3-C9682EC1275D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1BA0CD9A-B9E0-48D4-86D3-C9682EC1275D}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="70">
   <si>
     <t>Daily Scrum</t>
   </si>
@@ -230,7 +230,34 @@
 </t>
   </si>
   <si>
-    <t>The team discussed the separation of tasks for the remainder of the sprint, including reviewing commitments and setting realistic deadlines. We also addressed any concerns with task timing and how to leverage context for a more organized workflow.</t>
+    <t>NO MEETING</t>
+  </si>
+  <si>
+    <t>October 4rd, 2024</t>
+  </si>
+  <si>
+    <t>October 6th, 2024</t>
+  </si>
+  <si>
+    <t>October 10th, 2024</t>
+  </si>
+  <si>
+    <t>October 12th, 2024</t>
+  </si>
+  <si>
+    <t>October 20th, 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The team discussed the separation of tasks for the remainder of the sprint, including reviewing commitments and setting realistic deadlines. We also addressed any concerns with task timing and how to leverage context for a more organized workflow. </t>
+  </si>
+  <si>
+    <t>October 25th, 2024</t>
+  </si>
+  <si>
+    <t>October 26th, 2024</t>
+  </si>
+  <si>
+    <t>October 27th, 2024</t>
   </si>
 </sst>
 </file>
@@ -594,10 +621,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0ADACE44-A1BC-47E6-A04D-E724ACE2BBAC}">
-  <dimension ref="A1:J100"/>
+  <dimension ref="A1:J105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D13" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -654,25 +681,17 @@
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
     </row>
-    <row r="3" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>11</v>
+        <v>61</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>48</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="2"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
@@ -680,10 +699,10 @@
     </row>
     <row r="4" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>12</v>
@@ -692,35 +711,27 @@
         <v>9</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
     </row>
-    <row r="5" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>19</v>
+        <v>62</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>52</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
@@ -728,7 +739,7 @@
     </row>
     <row r="6" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>33</v>
@@ -740,10 +751,10 @@
         <v>9</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
@@ -752,10 +763,10 @@
     </row>
     <row r="7" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>12</v>
@@ -764,22 +775,22 @@
         <v>9</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
     </row>
-    <row r="8" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>12</v>
@@ -787,95 +798,79 @@
       <c r="D8" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>24</v>
+      <c r="E8" s="2" t="s">
+        <v>15</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
     </row>
-    <row r="9" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>25</v>
+        <v>63</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>54</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="C9" s="1"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
     </row>
-    <row r="10" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
     </row>
-    <row r="11" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>30</v>
+        <v>64</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>56</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="C11" s="1"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
     </row>
-    <row r="12" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>12</v>
@@ -883,23 +878,23 @@
       <c r="D12" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E12" s="2" t="s">
-        <v>39</v>
+      <c r="E12" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
     </row>
-    <row r="13" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>12</v>
@@ -908,10 +903,10 @@
         <v>9</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
@@ -920,67 +915,83 @@
     </row>
     <row r="14" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
     </row>
-    <row r="15" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
+    <row r="16" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>57</v>
+      </c>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
+      <c r="A17" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>60</v>
+      </c>
       <c r="C17" s="1"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
@@ -990,44 +1001,82 @@
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
+    <row r="18" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>58</v>
+      </c>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
+    <row r="19" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>59</v>
+      </c>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
+    <row r="20" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>66</v>
+      </c>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A21" s="1"/>
+      <c r="A21" s="1" t="s">
+        <v>67</v>
+      </c>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="2"/>
@@ -1039,7 +1088,9 @@
       <c r="J21" s="1"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A22" s="1"/>
+      <c r="A22" s="1" t="s">
+        <v>68</v>
+      </c>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="2"/>
@@ -1051,7 +1102,9 @@
       <c r="J22" s="1"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A23" s="1"/>
+      <c r="A23" s="1" t="s">
+        <v>69</v>
+      </c>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="2"/>
@@ -1078,9 +1131,9 @@
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
@@ -1090,9 +1143,9 @@
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
@@ -1102,9 +1155,9 @@
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
@@ -1114,8 +1167,9 @@
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
@@ -1125,9 +1179,9 @@
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
@@ -1173,7 +1227,6 @@
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
-      <c r="D33" s="1"/>
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
@@ -1985,6 +2038,66 @@
       <c r="I100" s="1"/>
       <c r="J100" s="1"/>
     </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A101" s="1"/>
+      <c r="B101" s="1"/>
+      <c r="C101" s="1"/>
+      <c r="D101" s="1"/>
+      <c r="E101" s="1"/>
+      <c r="F101" s="1"/>
+      <c r="G101" s="1"/>
+      <c r="H101" s="1"/>
+      <c r="I101" s="1"/>
+      <c r="J101" s="1"/>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A102" s="1"/>
+      <c r="B102" s="1"/>
+      <c r="C102" s="1"/>
+      <c r="D102" s="1"/>
+      <c r="E102" s="1"/>
+      <c r="F102" s="1"/>
+      <c r="G102" s="1"/>
+      <c r="H102" s="1"/>
+      <c r="I102" s="1"/>
+      <c r="J102" s="1"/>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A103" s="1"/>
+      <c r="B103" s="1"/>
+      <c r="C103" s="1"/>
+      <c r="D103" s="1"/>
+      <c r="E103" s="1"/>
+      <c r="F103" s="1"/>
+      <c r="G103" s="1"/>
+      <c r="H103" s="1"/>
+      <c r="I103" s="1"/>
+      <c r="J103" s="1"/>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A104" s="1"/>
+      <c r="B104" s="1"/>
+      <c r="C104" s="1"/>
+      <c r="D104" s="1"/>
+      <c r="E104" s="1"/>
+      <c r="F104" s="1"/>
+      <c r="G104" s="1"/>
+      <c r="H104" s="1"/>
+      <c r="I104" s="1"/>
+      <c r="J104" s="1"/>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A105" s="1"/>
+      <c r="B105" s="1"/>
+      <c r="C105" s="1"/>
+      <c r="D105" s="1"/>
+      <c r="E105" s="1"/>
+      <c r="F105" s="1"/>
+      <c r="G105" s="1"/>
+      <c r="H105" s="1"/>
+      <c r="I105" s="1"/>
+      <c r="J105" s="1"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>